<commit_message>
Backup QR Scanner data - 04/05/2025, 5:24:50 PM
</commit_message>
<xml_diff>
--- a/backups/Scanner_Biochemistry_Lab_2025-05-04T14-01-55.xlsx
+++ b/backups/Scanner_Biochemistry_Lab_2025-05-04T14-01-55.xlsx
@@ -397,54 +397,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Number</v>
+        <v>Student ID</v>
       </c>
       <c r="B1" t="str">
-        <v>Content</v>
+        <v>Location</v>
       </c>
       <c r="C1" t="str">
-        <v>Location</v>
+        <v>Log Date</v>
       </c>
       <c r="D1" t="str">
-        <v>Log Date</v>
+        <v>Log Time</v>
       </c>
       <c r="E1" t="str">
-        <v>Log Time</v>
-      </c>
-      <c r="F1" t="str">
         <v>Type</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="str">
+        <v>Gg</v>
       </c>
       <c r="B2" t="str">
-        <v>Gg</v>
+        <v>Biochemistry Lab</v>
       </c>
       <c r="C2" t="str">
-        <v>Biochemistry Lab</v>
+        <v>05/04/2025</v>
       </c>
       <c r="D2" t="str">
-        <v>05/04/2025</v>
+        <v>5:01 PM</v>
       </c>
       <c r="E2" t="str">
-        <v>5:01 PM</v>
-      </c>
-      <c r="F2" t="str">
         <v>Manual</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>